<commit_message>
giao dien 3 chuc nang PM,update DB
</commit_message>
<xml_diff>
--- a/CM_Plan/Requirement/URD/WLS_URD_v0.1_EN.xlsx
+++ b/CM_Plan/Requirement/URD/WLS_URD_v0.1_EN.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView windowWidth="28200" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -69,6 +69,9 @@
     <t>Use different types of charts when making statistical functions</t>
   </si>
   <si>
+    <t>There is a multi-day work log function for members to quickly declare, for repetitive tasks over days</t>
+  </si>
+  <si>
     <t>The work log after the member has been created, the system will approve it by default</t>
   </si>
   <si>
@@ -82,21 +85,24 @@
   </si>
   <si>
     <t>There is a product named Meeting, the conductor will declare as Create, the person who writes the minutes of the meeting will declare as Create, the meeting participant  will declare as Review / Test for this product.</t>
-  </si>
-  <si>
-    <t>There is a multi-day work log function for members to quickly declare, for repetitive tasks over days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -104,19 +110,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -124,19 +467,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -427,30 +1059,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B2:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="3.08984375" customWidth="1"/>
+    <col min="2" max="2" width="3.09166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -458,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -466,7 +1098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -474,7 +1106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -482,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -490,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -498,7 +1130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -506,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -514,7 +1146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -522,7 +1154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -530,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14">
         <v>11</v>
       </c>
@@ -538,7 +1170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15">
         <v>12</v>
       </c>
@@ -546,7 +1178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16">
         <v>13</v>
       </c>
@@ -554,7 +1186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17">
         <v>14</v>
       </c>
@@ -562,7 +1194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3">
       <c r="B18">
         <v>15</v>
       </c>
@@ -570,7 +1202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3">
       <c r="B19">
         <v>16</v>
       </c>
@@ -578,52 +1210,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3">
       <c r="B20">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
       <c r="B21">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
       <c r="B23">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
       <c r="B24">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
       <c r="B25">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>